<commit_message>
metre unité des axes Des titres
</commit_message>
<xml_diff>
--- a/gyro.xlsx
+++ b/gyro.xlsx
@@ -379,7 +379,7 @@
         <v>43294.64785653936</v>
       </c>
       <c r="C2">
-        <v>8974.119678274856</v>
+        <v>68.51069550467862</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -390,7 +390,7 @@
         <v>43294.81463670139</v>
       </c>
       <c r="C3">
-        <v>2858.968345400137</v>
+        <v>21.82653231970764</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -401,7 +401,7 @@
         <v>43294.8982940162</v>
       </c>
       <c r="C4">
-        <v>2204.209835746134</v>
+        <v>16.82898451760796</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -412,7 +412,7 @@
         <v>43294.98195237268</v>
       </c>
       <c r="C5">
-        <v>2525.201576112291</v>
+        <v>19.27929813997132</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -423,7 +423,7 @@
         <v>43295.06565225695</v>
       </c>
       <c r="C6">
-        <v>2751.103960231238</v>
+        <v>20.99778258680033</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -434,7 +434,7 @@
         <v>43295.23268549769</v>
       </c>
       <c r="C7">
-        <v>2603.877301256724</v>
+        <v>19.87336833044948</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -445,7 +445,7 @@
         <v>43295.31634289351</v>
       </c>
       <c r="C8">
-        <v>2746.315531762511</v>
+        <v>20.96114401019804</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -456,7 +456,7 @@
         <v>43295.4000008912</v>
       </c>
       <c r="C9">
-        <v>5258.369614243563</v>
+        <v>40.13926791400924</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -467,7 +467,7 @@
         <v>43295.48365900463</v>
       </c>
       <c r="C10">
-        <v>2565.283999872139</v>
+        <v>19.57925294315347</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -478,7 +478,7 @@
         <v>43295.56731715277</v>
       </c>
       <c r="C11">
-        <v>2464.376797488566</v>
+        <v>18.80933322616883</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -489,7 +489,7 @@
         <v>43295.65097576389</v>
       </c>
       <c r="C12">
-        <v>6567.476075327569</v>
+        <v>50.13508493338818</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -500,7 +500,7 @@
         <v>43295.85976931713</v>
       </c>
       <c r="C13">
-        <v>9849.668471578118</v>
+        <v>75.18997545363945</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -511,7 +511,7 @@
         <v>43295.98522641203</v>
       </c>
       <c r="C14">
-        <v>3910.580135990055</v>
+        <v>29.85440282233725</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -522,7 +522,7 @@
         <v>43296.06897854167</v>
       </c>
       <c r="C15">
-        <v>2269.005068306371</v>
+        <v>17.32348595983144</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -533,7 +533,7 @@
         <v>43296.1526362037</v>
       </c>
       <c r="C16">
-        <v>3538.182866953035</v>
+        <v>27.01260237527866</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -544,7 +544,7 @@
         <v>43296.23629368056</v>
       </c>
       <c r="C17">
-        <v>2351.005316880419</v>
+        <v>17.95003522569893</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -555,7 +555,7 @@
         <v>43296.31995261574</v>
       </c>
       <c r="C18">
-        <v>2878.86418575104</v>
+        <v>21.97876526869545</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -566,7 +566,7 @@
         <v>43296.40362675926</v>
       </c>
       <c r="C19">
-        <v>2097.399580432875</v>
+        <v>16.01351002719738</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -577,7 +577,7 @@
         <v>43296.57069726852</v>
       </c>
       <c r="C20">
-        <v>4130.421407072165</v>
+        <v>31.53190461125791</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -588,7 +588,7 @@
         <v>43296.73778114584</v>
       </c>
       <c r="C21">
-        <v>3094.450031911971</v>
+        <v>23.6246319181533</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -599,7 +599,7 @@
         <v>43296.82150574074</v>
       </c>
       <c r="C22">
-        <v>6333.940479669824</v>
+        <v>48.35025437515775</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -610,7 +610,7 @@
         <v>43296.90519020833</v>
       </c>
       <c r="C23">
-        <v>2413.936204625134</v>
+        <v>18.42986517649373</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -621,7 +621,7 @@
         <v>43296.98884871528</v>
       </c>
       <c r="C24">
-        <v>4081.323682336406</v>
+        <v>31.15820353891376</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -632,7 +632,7 @@
         <v>43297.07250678241</v>
       </c>
       <c r="C25">
-        <v>3551.97677357271</v>
+        <v>27.11105586389386</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -643,7 +643,7 @@
         <v>43297.15628873843</v>
       </c>
       <c r="C26">
-        <v>3173.646640695842</v>
+        <v>24.22353528893922</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -654,7 +654,7 @@
         <v>43297.32340094908</v>
       </c>
       <c r="C27">
-        <v>1946.906777429263</v>
+        <v>14.8590160221776</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -665,7 +665,7 @@
         <v>43297.4071402662</v>
       </c>
       <c r="C28">
-        <v>3061.86642425825</v>
+        <v>23.36979170070383</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -676,7 +676,7 @@
         <v>43297.49079854166</v>
       </c>
       <c r="C29">
-        <v>2041.113666604582</v>
+        <v>15.5782255349262</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -687,7 +687,7 @@
         <v>43297.57445674769</v>
       </c>
       <c r="C30">
-        <v>4844.581406065957</v>
+        <v>36.97846604231074</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -698,7 +698,7 @@
         <v>43297.65811539352</v>
       </c>
       <c r="C31">
-        <v>3971.196545123396</v>
+        <v>30.31328650246572</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -709,7 +709,7 @@
         <v>43297.74177369213</v>
       </c>
       <c r="C32">
-        <v>2360.048516450456</v>
+        <v>18.01285210148267</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -720,7 +720,7 @@
         <v>43297.82547327546</v>
       </c>
       <c r="C33">
-        <v>8298.124727912927</v>
+        <v>63.34770635079018</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -731,7 +731,7 @@
         <v>43297.99259774305</v>
       </c>
       <c r="C34">
-        <v>2875.798845538401</v>
+        <v>21.95497997601598</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -742,7 +742,7 @@
         <v>43298.07625605324</v>
       </c>
       <c r="C35">
-        <v>3924.23317350027</v>
+        <v>29.9528313633764</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -753,7 +753,7 @@
         <v>43298.15991417824</v>
       </c>
       <c r="C36">
-        <v>2180.700804787305</v>
+        <v>16.64932322838625</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -764,7 +764,7 @@
         <v>43298.24357263889</v>
       </c>
       <c r="C37">
-        <v>4478.635841414213</v>
+        <v>34.19079165018652</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -775,7 +775,7 @@
         <v>43298.36900363426</v>
       </c>
       <c r="C38">
-        <v>2291.159968225702</v>
+        <v>17.4926721642098</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -786,7 +786,7 @@
         <v>43298.45274141204</v>
       </c>
       <c r="C39">
-        <v>2653.758466778768</v>
+        <v>20.26149678069221</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -797,7 +797,7 @@
         <v>43298.49473298611</v>
       </c>
       <c r="C40">
-        <v>3038.490085552362</v>
+        <v>23.19170883719455</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -808,7 +808,7 @@
         <v>43298.53672443287</v>
       </c>
       <c r="C41">
-        <v>2563.209901666268</v>
+        <v>19.56377635882729</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -819,7 +819,7 @@
         <v>43298.56638480324</v>
       </c>
       <c r="C42">
-        <v>5639.955850891033</v>
+        <v>43.05058324576986</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrections suite essai chez Moet : - Modif calcul Rotation (roulis) - hausse du seuil de détection du mouvement
</commit_message>
<xml_diff>
--- a/gyro.xlsx
+++ b/gyro.xlsx
@@ -354,7 +354,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -373,453 +373,442 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>43294.64785653936</v>
+        <v>44016.01101173611</v>
       </c>
       <c r="B2">
-        <v>43294.64785653936</v>
+        <v>44016.01101173611</v>
       </c>
       <c r="C2">
-        <v>68.51069550467862</v>
+        <v>18.80551484962127</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>43294.81463670139</v>
+        <v>44016.13601262731</v>
       </c>
       <c r="B3">
-        <v>43294.81463670139</v>
+        <v>44016.13601262731</v>
       </c>
       <c r="C3">
-        <v>21.82653231970764</v>
+        <v>15.57982196646137</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>43294.8982940162</v>
+        <v>44016.26101241898</v>
       </c>
       <c r="B4">
-        <v>43294.8982940162</v>
+        <v>44016.26101241898</v>
       </c>
       <c r="C4">
-        <v>16.82898451760796</v>
+        <v>19.46270824064371</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>43294.98195237268</v>
+        <v>44016.38601284722</v>
       </c>
       <c r="B5">
-        <v>43294.98195237268</v>
+        <v>44016.38601284722</v>
       </c>
       <c r="C5">
-        <v>19.27929813997132</v>
+        <v>18.2398743872448</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
-        <v>43295.06565225695</v>
+        <v>44016.46934637731</v>
       </c>
       <c r="B6">
-        <v>43295.06565225695</v>
+        <v>44016.46934637731</v>
       </c>
       <c r="C6">
-        <v>20.99778258680033</v>
+        <v>16.7297456755481</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>43295.23268549769</v>
+        <v>44016.55268054398</v>
       </c>
       <c r="B7">
-        <v>43295.23268549769</v>
+        <v>44016.55268054398</v>
       </c>
       <c r="C7">
-        <v>19.87336833044948</v>
+        <v>19.07880620574052</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>43295.31634289351</v>
+        <v>44016.63601412037</v>
       </c>
       <c r="B8">
-        <v>43295.31634289351</v>
+        <v>44016.63601412037</v>
       </c>
       <c r="C8">
-        <v>20.96114401019804</v>
+        <v>18.9453468946629</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9">
-        <v>43295.4000008912</v>
+        <v>44016.71934768518</v>
       </c>
       <c r="B9">
-        <v>43295.4000008912</v>
+        <v>44016.71934768518</v>
       </c>
       <c r="C9">
-        <v>40.13926791400924</v>
+        <v>15.4221518268304</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
-        <v>43295.48365900463</v>
+        <v>44016.8026812963</v>
       </c>
       <c r="B10">
-        <v>43295.48365900463</v>
+        <v>44016.8026812963</v>
       </c>
       <c r="C10">
-        <v>19.57925294315347</v>
+        <v>14.12743757087701</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11">
-        <v>43295.56731715277</v>
+        <v>44016.88601451389</v>
       </c>
       <c r="B11">
-        <v>43295.56731715277</v>
+        <v>44016.88601451389</v>
       </c>
       <c r="C11">
-        <v>18.80933322616883</v>
+        <v>11.64253309010407</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12">
-        <v>43295.65097576389</v>
+        <v>44016.96934958333</v>
       </c>
       <c r="B12">
-        <v>43295.65097576389</v>
+        <v>44016.96934958333</v>
       </c>
       <c r="C12">
-        <v>50.13508493338818</v>
+        <v>19.10189268745386</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13">
-        <v>43295.85976931713</v>
+        <v>44017.05268149306</v>
       </c>
       <c r="B13">
-        <v>43295.85976931713</v>
+        <v>44017.05268149306</v>
       </c>
       <c r="C13">
-        <v>75.18997545363945</v>
+        <v>20.18016234122768</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14">
-        <v>43295.98522641203</v>
+        <v>44017.09434935185</v>
       </c>
       <c r="B14">
-        <v>43295.98522641203</v>
+        <v>44017.09434935185</v>
       </c>
       <c r="C14">
-        <v>29.85440282233725</v>
+        <v>17.32925357398156</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15">
-        <v>43296.06897854167</v>
+        <v>44017.13601577546</v>
       </c>
       <c r="B15">
-        <v>43296.06897854167</v>
+        <v>44017.13601577546</v>
       </c>
       <c r="C15">
-        <v>17.32348595983144</v>
+        <v>17.29736557213202</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16">
-        <v>43296.1526362037</v>
+        <v>44017.17768247685</v>
       </c>
       <c r="B16">
-        <v>43296.1526362037</v>
+        <v>44017.17768247685</v>
       </c>
       <c r="C16">
-        <v>27.01260237527866</v>
+        <v>14.78937019265054</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17">
-        <v>43296.23629368056</v>
+        <v>44017.21934922454</v>
       </c>
       <c r="B17">
-        <v>43296.23629368056</v>
+        <v>44017.21934922454</v>
       </c>
       <c r="C17">
-        <v>17.95003522569893</v>
+        <v>12.96392668670762</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18">
-        <v>43296.31995261574</v>
+        <v>44017.26101645833</v>
       </c>
       <c r="B18">
-        <v>43296.31995261574</v>
+        <v>44017.26101645833</v>
       </c>
       <c r="C18">
-        <v>21.97876526869545</v>
+        <v>17.06014353734072</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19">
-        <v>43296.40362675926</v>
+        <v>44017.34435050926</v>
       </c>
       <c r="B19">
-        <v>43296.40362675926</v>
+        <v>44017.34435050926</v>
       </c>
       <c r="C19">
-        <v>16.01351002719738</v>
+        <v>19.32721592894027</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20">
-        <v>43296.57069726852</v>
+        <v>44017.36518381944</v>
       </c>
       <c r="B20">
-        <v>43296.57069726852</v>
+        <v>44017.36518381944</v>
       </c>
       <c r="C20">
-        <v>31.53190461125791</v>
+        <v>18.28503239591587</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21">
-        <v>43296.73778114584</v>
+        <v>44017.38601743056</v>
       </c>
       <c r="B21">
-        <v>43296.73778114584</v>
+        <v>44017.38601743056</v>
       </c>
       <c r="C21">
-        <v>23.6246319181533</v>
+        <v>14.78444079222214</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22">
-        <v>43296.82150574074</v>
+        <v>44017.4068509838</v>
       </c>
       <c r="B22">
-        <v>43296.82150574074</v>
+        <v>44017.4068509838</v>
       </c>
       <c r="C22">
-        <v>48.35025437515775</v>
+        <v>13.61043070325539</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23">
-        <v>43296.90519020833</v>
+        <v>44017.42768402777</v>
       </c>
       <c r="B23">
-        <v>43296.90519020833</v>
+        <v>44017.42768402777</v>
       </c>
       <c r="C23">
-        <v>18.42986517649373</v>
+        <v>12.47544836088552</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24">
-        <v>43296.98884871528</v>
+        <v>44017.44851708334</v>
       </c>
       <c r="B24">
-        <v>43296.98884871528</v>
+        <v>44017.44851708334</v>
       </c>
       <c r="C24">
-        <v>31.15820353891376</v>
+        <v>11.88504043425403</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25">
-        <v>43297.07250678241</v>
+        <v>44017.46935116898</v>
       </c>
       <c r="B25">
-        <v>43297.07250678241</v>
+        <v>44017.46935116898</v>
       </c>
       <c r="C25">
-        <v>27.11105586389386</v>
+        <v>13.07926754730207</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26">
-        <v>43297.15628873843</v>
+        <v>44017.49018402777</v>
       </c>
       <c r="B26">
-        <v>43297.15628873843</v>
+        <v>44017.49018402777</v>
       </c>
       <c r="C26">
-        <v>24.22353528893922</v>
+        <v>18.27943959873594</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27">
-        <v>43297.32340094908</v>
+        <v>44017.51101752315</v>
       </c>
       <c r="B27">
-        <v>43297.32340094908</v>
+        <v>44017.51101752315</v>
       </c>
       <c r="C27">
-        <v>14.8590160221776</v>
+        <v>18.8105504946702</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28">
-        <v>43297.4071402662</v>
+        <v>44017.53185171296</v>
       </c>
       <c r="B28">
-        <v>43297.4071402662</v>
+        <v>44017.53185171296</v>
       </c>
       <c r="C28">
-        <v>23.36979170070383</v>
+        <v>20.93276519338268</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29">
-        <v>43297.49079854166</v>
+        <v>44017.55268495371</v>
       </c>
       <c r="B29">
-        <v>43297.49079854166</v>
+        <v>44017.55268495371</v>
       </c>
       <c r="C29">
-        <v>15.5782255349262</v>
+        <v>18.26734424055163</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30">
-        <v>43297.57445674769</v>
+        <v>44017.57351759259</v>
       </c>
       <c r="B30">
-        <v>43297.57445674769</v>
+        <v>44017.57351759259</v>
       </c>
       <c r="C30">
-        <v>36.97846604231074</v>
+        <v>14.269456528228</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31">
-        <v>43297.65811539352</v>
+        <v>44017.59435203703</v>
       </c>
       <c r="B31">
-        <v>43297.65811539352</v>
+        <v>44017.59435203703</v>
       </c>
       <c r="C31">
-        <v>30.31328650246572</v>
+        <v>15.09481957186472</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32">
-        <v>43297.74177369213</v>
+        <v>44017.61518556713</v>
       </c>
       <c r="B32">
-        <v>43297.74177369213</v>
+        <v>44017.61518556713</v>
       </c>
       <c r="C32">
-        <v>18.01285210148267</v>
+        <v>13.74438795180833</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33">
-        <v>43297.82547327546</v>
+        <v>44017.63601891204</v>
       </c>
       <c r="B33">
-        <v>43297.82547327546</v>
+        <v>44017.63601891204</v>
       </c>
       <c r="C33">
-        <v>63.34770635079018</v>
+        <v>15.31706305991288</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34">
-        <v>43297.99259774305</v>
+        <v>44017.65685251157</v>
       </c>
       <c r="B34">
-        <v>43297.99259774305</v>
+        <v>44017.65685251157</v>
       </c>
       <c r="C34">
-        <v>21.95497997601598</v>
+        <v>14.50166824687897</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35">
-        <v>43298.07625605324</v>
+        <v>44017.67768590278</v>
       </c>
       <c r="B35">
-        <v>43298.07625605324</v>
+        <v>44017.67768590278</v>
       </c>
       <c r="C35">
-        <v>29.9528313633764</v>
+        <v>18.87703936306888</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36">
-        <v>43298.15991417824</v>
+        <v>44017.69851924769</v>
       </c>
       <c r="B36">
-        <v>43298.15991417824</v>
+        <v>44017.69851924769</v>
       </c>
       <c r="C36">
-        <v>16.64932322838625</v>
+        <v>19.39444178700686</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37">
-        <v>43298.24357263889</v>
+        <v>44017.71935284722</v>
       </c>
       <c r="B37">
-        <v>43298.24357263889</v>
+        <v>44017.71935284722</v>
       </c>
       <c r="C37">
-        <v>34.19079165018652</v>
+        <v>18.22805576955546</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38">
-        <v>43298.36900363426</v>
+        <v>44017.74018612268</v>
       </c>
       <c r="B38">
-        <v>43298.36900363426</v>
+        <v>44017.74018612268</v>
       </c>
       <c r="C38">
-        <v>17.4926721642098</v>
+        <v>17.30990101423312</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39">
-        <v>43298.45274141204</v>
+        <v>44017.76101953704</v>
       </c>
       <c r="B39">
-        <v>43298.45274141204</v>
+        <v>44017.76101953704</v>
       </c>
       <c r="C39">
-        <v>20.26149678069221</v>
+        <v>13.9500873976135</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40">
-        <v>43298.49473298611</v>
+        <v>44017.78185297453</v>
       </c>
       <c r="B40">
-        <v>43298.49473298611</v>
+        <v>44017.78185297453</v>
       </c>
       <c r="C40">
-        <v>23.19170883719455</v>
+        <v>13.10761160536024</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41">
-        <v>43298.53672443287</v>
+        <v>44017.80268631945</v>
       </c>
       <c r="B41">
-        <v>43298.53672443287</v>
+        <v>44017.80268631945</v>
       </c>
       <c r="C41">
-        <v>19.56377635882729</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42">
-        <v>43298.56638480324</v>
-      </c>
-      <c r="B42">
-        <v>43298.56638480324</v>
-      </c>
-      <c r="C42">
-        <v>43.05058324576986</v>
+        <v>18.6711505101691</v>
       </c>
     </row>
   </sheetData>

</xml_diff>